<commit_message>
Ajout d'une 12ème place pour le Champidrome (test commit)
</commit_message>
<xml_diff>
--- a/Courses_mk8.xlsx
+++ b/Courses_mk8.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/051213282364fe6a/Documents/Projets_perso/projet_MK8/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u.devoille\OneDrive - Systancia\Documents\projet-perso\Projet-MK8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{DFD8C933-F445-45B1-8BCC-C75EFDFBF1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C18C6E40-1458-4BA4-B0CE-CAE4DC663C8E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F45C5D1-CE46-4CBF-928C-C4878B6777B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Courses_mario_kart" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="100">
   <si>
     <t>Champidrome</t>
   </si>
@@ -923,21 +923,21 @@
   <dimension ref="A1:P65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K32" sqref="K32"/>
+      <selection pane="bottomRight" activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.1796875" customWidth="1"/>
-    <col min="2" max="3" width="10.453125" customWidth="1"/>
-    <col min="4" max="4" width="19.1796875" customWidth="1"/>
-    <col min="5" max="16" width="8.54296875" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="16" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>80</v>
       </c>
@@ -987,7 +987,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1033,11 +1033,11 @@
       <c r="O2" s="5">
         <v>1</v>
       </c>
-      <c r="P2" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1085,7 +1085,7 @@
       </c>
       <c r="P3" s="5"/>
     </row>
-    <row r="4" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="P4" s="5"/>
     </row>
-    <row r="5" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="P5" s="5"/>
     </row>
-    <row r="6" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1277,7 +1277,7 @@
       </c>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1325,7 +1325,7 @@
       </c>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="P10" s="5"/>
     </row>
-    <row r="11" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="P12" s="5"/>
     </row>
-    <row r="13" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="P14" s="5"/>
     </row>
-    <row r="15" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1665,7 +1665,7 @@
       </c>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="P16" s="5"/>
     </row>
-    <row r="17" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="P18" s="5"/>
     </row>
-    <row r="19" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="P19" s="5"/>
     </row>
-    <row r="20" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -1907,7 +1907,7 @@
       </c>
       <c r="P20" s="5"/>
     </row>
-    <row r="21" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -1955,7 +1955,7 @@
       </c>
       <c r="P21" s="5"/>
     </row>
-    <row r="22" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -2053,7 +2053,7 @@
       </c>
       <c r="P23" s="5"/>
     </row>
-    <row r="24" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="P24" s="5"/>
     </row>
-    <row r="25" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -2149,7 +2149,7 @@
       </c>
       <c r="P25" s="5"/>
     </row>
-    <row r="26" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -2197,7 +2197,7 @@
       </c>
       <c r="P26" s="5"/>
     </row>
-    <row r="27" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -2245,7 +2245,7 @@
       </c>
       <c r="P27" s="5"/>
     </row>
-    <row r="28" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -2293,7 +2293,7 @@
       </c>
       <c r="P28" s="5"/>
     </row>
-    <row r="29" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
@@ -2341,7 +2341,7 @@
       </c>
       <c r="P29" s="5"/>
     </row>
-    <row r="30" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
@@ -2539,7 +2539,7 @@
       </c>
       <c r="P33" s="5"/>
     </row>
-    <row r="34" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
@@ -2687,7 +2687,7 @@
       </c>
       <c r="P36" s="5"/>
     </row>
-    <row r="37" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
@@ -2785,7 +2785,7 @@
       </c>
       <c r="P38" s="5"/>
     </row>
-    <row r="39" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
@@ -2833,7 +2833,7 @@
       </c>
       <c r="P39" s="5"/>
     </row>
-    <row r="40" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
@@ -2881,7 +2881,7 @@
       </c>
       <c r="P40" s="5"/>
     </row>
-    <row r="41" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
@@ -2929,7 +2929,7 @@
       </c>
       <c r="P41" s="5"/>
     </row>
-    <row r="42" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
@@ -2977,7 +2977,7 @@
       </c>
       <c r="P42" s="5"/>
     </row>
-    <row r="43" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="P43" s="5"/>
     </row>
-    <row r="44" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
@@ -3123,7 +3123,7 @@
       </c>
       <c r="P45" s="5"/>
     </row>
-    <row r="46" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
@@ -3171,7 +3171,7 @@
       </c>
       <c r="P46" s="5"/>
     </row>
-    <row r="47" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
@@ -3217,7 +3217,7 @@
       </c>
       <c r="P47" s="5"/>
     </row>
-    <row r="48" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
@@ -3315,7 +3315,7 @@
       </c>
       <c r="P49" s="5"/>
     </row>
-    <row r="50" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -3347,7 +3347,7 @@
       <c r="O50" s="6"/>
       <c r="P50" s="5"/>
     </row>
-    <row r="51" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="P51" s="5"/>
     </row>
-    <row r="52" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -3411,7 +3411,7 @@
       </c>
       <c r="P52" s="5"/>
     </row>
-    <row r="53" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -3443,7 +3443,7 @@
       </c>
       <c r="P53" s="5"/>
     </row>
-    <row r="54" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -3479,7 +3479,7 @@
       <c r="O54" s="6"/>
       <c r="P54" s="5"/>
     </row>
-    <row r="55" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -3515,7 +3515,7 @@
       <c r="O55" s="6"/>
       <c r="P55" s="5"/>
     </row>
-    <row r="56" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -3553,7 +3553,7 @@
       <c r="O56" s="6"/>
       <c r="P56" s="5"/>
     </row>
-    <row r="57" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -3581,7 +3581,7 @@
       <c r="O57" s="6"/>
       <c r="P57" s="5"/>
     </row>
-    <row r="58" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>90</v>
       </c>
@@ -3611,7 +3611,7 @@
       <c r="O58" s="7"/>
       <c r="P58" s="8"/>
     </row>
-    <row r="59" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>91</v>
       </c>
@@ -3645,7 +3645,7 @@
       <c r="O59" s="7"/>
       <c r="P59" s="8"/>
     </row>
-    <row r="60" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>92</v>
       </c>
@@ -3675,7 +3675,7 @@
       <c r="O60" s="7"/>
       <c r="P60" s="8"/>
     </row>
-    <row r="61" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>93</v>
       </c>
@@ -3701,7 +3701,7 @@
       <c r="O61" s="7"/>
       <c r="P61" s="8"/>
     </row>
-    <row r="62" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>94</v>
       </c>
@@ -3731,7 +3731,7 @@
       <c r="O62" s="7"/>
       <c r="P62" s="8"/>
     </row>
-    <row r="63" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>95</v>
       </c>
@@ -3761,7 +3761,7 @@
       <c r="O63" s="7"/>
       <c r="P63" s="7"/>
     </row>
-    <row r="64" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>96</v>
       </c>
@@ -3791,7 +3791,7 @@
       <c r="O64" s="7"/>
       <c r="P64" s="7"/>
     </row>
-    <row r="65" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>97</v>
       </c>

</xml_diff>

<commit_message>
troisième commit de test
</commit_message>
<xml_diff>
--- a/Courses_mk8.xlsx
+++ b/Courses_mk8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u.devoille\OneDrive - Systancia\Documents\projet-perso\Projet-MK8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F45C5D1-CE46-4CBF-928C-C4878B6777B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BF9074-8F80-4F5C-BB8D-D7FAAC3A4513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -926,7 +926,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q7" sqref="Q7"/>
+      <selection pane="bottomRight" activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1033,9 +1033,7 @@
       <c r="O2" s="5">
         <v>1</v>
       </c>
-      <c r="P2" s="5">
-        <v>1</v>
-      </c>
+      <c r="P2" s="5"/>
     </row>
     <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">

</xml_diff>